<commit_message>
update excel sheet to run from jenkins
</commit_message>
<xml_diff>
--- a/DataDrivenMaven/src/test/java/testData/TestData.xlsx
+++ b/DataDrivenMaven/src/test/java/testData/TestData.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <workbookPr defaultThemeVersion="124226" filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView windowHeight="8010" windowWidth="14805" xWindow="240" yWindow="105"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet1" r:id="rId1" sheetId="1"/>
+    <sheet name="Sheet2" r:id="rId2" sheetId="2"/>
+    <sheet name="Sheet3" r:id="rId3" sheetId="3"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="34">
   <si>
     <t>Test Case Name</t>
   </si>
@@ -200,28 +200,28 @@
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="7">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="1"/>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" quotePrefix="1" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="2" fillId="2" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf applyBorder="1" applyFill="1" borderId="2" fillId="0" fontId="2" numFmtId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleMedium9" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -238,10 +238,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -276,7 +276,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin panose="020F0302020204030204" typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -311,7 +311,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -399,7 +399,7 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="95000"/>
@@ -408,13 +408,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -424,7 +424,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -433,7 +433,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -442,7 +442,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -452,12 +452,12 @@
             <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
+            <a:lightRig dir="t" rig="threePt">
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
+            <a:bevelT h="25400" w="63500"/>
           </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
@@ -488,7 +488,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+            <a:fillToRect b="180000" l="50000" r="50000" t="-80000"/>
           </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
@@ -507,7 +507,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+            <a:fillToRect b="50000" l="50000" r="50000" t="50000"/>
           </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
@@ -519,8 +519,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:O3"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <selection activeCell="M10" sqref="M10"/>
@@ -540,7 +540,7 @@
     <col min="13" max="13" bestFit="true" customWidth="true" width="20.0" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="30" r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -674,44 +674,44 @@
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E3">
+    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="E2:E3" type="list">
       <formula1>"Accessories, iMacs, iPads, iPhones"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F3">
+    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="F2:F3" type="list">
       <formula1>"Product 1, Product 2, Product 3, Product 4"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1"/>
-    <hyperlink ref="M2" r:id="rId2"/>
-    <hyperlink ref="C3" r:id="rId3"/>
-    <hyperlink ref="M3" r:id="rId4"/>
+    <hyperlink r:id="rId1" ref="C2"/>
+    <hyperlink r:id="rId2" ref="M2"/>
+    <hyperlink r:id="rId3" ref="C3"/>
+    <hyperlink r:id="rId4" ref="M3"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>